<commit_message>
updated table of accuracies and confusion matrices
</commit_message>
<xml_diff>
--- a/figures/Table of Accuracies.xlsx
+++ b/figures/Table of Accuracies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabiki\Desktop\development\schmitz_r-lymphocyte_activation\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E10F511-14D4-4232-89AA-CF123834CDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFD53AC-4341-4F6C-B365-8455A5264D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60705" yWindow="9330" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,19 +397,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.84375" customWidth="1"/>
-    <col min="3" max="3" width="41.3828125" customWidth="1"/>
-    <col min="4" max="4" width="10.61328125" bestFit="1"/>
-    <col min="10" max="10" width="11.765625" bestFit="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -476,7 +476,7 @@
         <v>0.63360881542699699</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -508,7 +508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -519,31 +519,31 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>0.99081726354453625</v>
+        <v>0.90723562152133497</v>
       </c>
       <c r="E4">
-        <v>0.88292011019283745</v>
+        <v>0.72634508348794002</v>
       </c>
       <c r="F4">
-        <v>0.94674012855831036</v>
+        <v>0.80612244897959096</v>
       </c>
       <c r="G4">
-        <v>0.96923783287419651</v>
+        <v>0.82745825602968404</v>
       </c>
       <c r="H4">
-        <v>0.97107438016528924</v>
+        <v>0.86456400742115003</v>
       </c>
       <c r="I4">
-        <v>0.95546372819100089</v>
+        <v>0.86456400742115003</v>
       </c>
       <c r="J4">
-        <v>0.54315886134067948</v>
+        <v>0.50927643784786603</v>
       </c>
       <c r="K4">
-        <v>0.80440771349862261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.56029684601113094</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -554,28 +554,28 @@
         <v>21</v>
       </c>
       <c r="D5">
-        <v>0.9173553719008265</v>
+        <v>0.86085343228200295</v>
       </c>
       <c r="E5">
-        <v>0.60835629017447201</v>
+        <v>0.36549165120593602</v>
       </c>
       <c r="F5">
-        <v>0.80991735537190079</v>
+        <v>0.62523191094619601</v>
       </c>
       <c r="G5">
-        <v>0.86225895316804413</v>
+        <v>0.76066790352504599</v>
       </c>
       <c r="H5">
-        <v>0.88705234159779611</v>
+        <v>0.81632653061224403</v>
       </c>
       <c r="I5">
-        <v>0.87235996326905418</v>
+        <v>0.77272727272727204</v>
       </c>
       <c r="J5">
-        <v>0.37741046831955921</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.34786641929499001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -586,28 +586,28 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>0.92745638200183655</v>
+        <v>0.92486085343228197</v>
       </c>
       <c r="E6">
-        <v>0.69513314967860418</v>
+        <v>0.67996289424860801</v>
       </c>
       <c r="F6">
-        <v>0.86179981634527092</v>
+        <v>0.84230055658627001</v>
       </c>
       <c r="G6">
-        <v>0.89072543617998168</v>
+        <v>0.87569573283859004</v>
       </c>
       <c r="H6">
-        <v>0.90679522497704312</v>
+        <v>0.90630797773654903</v>
       </c>
       <c r="I6">
-        <v>0.90541781450872361</v>
+        <v>0.90538033395176198</v>
       </c>
       <c r="J6">
-        <v>0.66574839302112032</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.60853432282003705</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -618,33 +618,33 @@
         <v>13</v>
       </c>
       <c r="D7">
-        <v>0.99068100358422939</v>
+        <v>0.89847715736040601</v>
       </c>
       <c r="E7">
-        <v>0.87813620071684584</v>
+        <v>0.75465313028764802</v>
       </c>
       <c r="F7">
-        <v>0.95483870967741935</v>
+        <v>0.81725888324873097</v>
       </c>
       <c r="G7">
-        <v>0.97347670250896057</v>
+        <v>0.85109983079526197</v>
       </c>
       <c r="H7">
-        <v>0.978494623655914</v>
+        <v>0.87817258883248706</v>
       </c>
       <c r="I7">
-        <v>0.96272401433691757</v>
+        <v>0.86971235194585395</v>
       </c>
       <c r="J7">
-        <v>0.59211469534050176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.50084602368866304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -679,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -719,7 +719,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -758,7 +758,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -770,38 +770,38 @@
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>99.081726354453622</v>
+        <v>90.723562152133496</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
-        <v>88.292011019283748</v>
+        <v>72.634508348794</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" ref="F16:K16" si="3">F4*100</f>
-        <v>94.674012855831037</v>
+        <v>80.612244897959101</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="3"/>
-        <v>96.923783287419653</v>
+        <v>82.745825602968409</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="3"/>
-        <v>97.107438016528931</v>
+        <v>86.456400742115008</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="3"/>
-        <v>95.546372819100085</v>
+        <v>86.456400742115008</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="3"/>
-        <v>54.315886134067945</v>
+        <v>50.927643784786603</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="3"/>
-        <v>80.44077134986226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+        <v>56.029684601113097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -813,35 +813,35 @@
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>91.735537190082653</v>
+        <v>86.085343228200301</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>60.835629017447204</v>
+        <v>36.549165120593599</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" ref="F17:J17" si="4">F5*100</f>
-        <v>80.991735537190081</v>
+        <v>62.523191094619598</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="4"/>
-        <v>86.225895316804412</v>
+        <v>76.066790352504597</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="4"/>
-        <v>88.705234159779607</v>
+        <v>81.632653061224403</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="4"/>
-        <v>87.235996326905422</v>
+        <v>77.272727272727209</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="4"/>
-        <v>37.74104683195592</v>
+        <v>34.786641929498998</v>
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -853,35 +853,35 @@
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>92.745638200183649</v>
+        <v>92.486085343228197</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>69.513314967860424</v>
+        <v>67.996289424860805</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ref="F18:J18" si="5">F6*100</f>
-        <v>86.179981634527095</v>
+        <v>84.230055658626995</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="5"/>
-        <v>89.072543617998164</v>
+        <v>87.569573283859</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="5"/>
-        <v>90.679522497704312</v>
+        <v>90.630797773654905</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="5"/>
-        <v>90.541781450872364</v>
+        <v>90.5380333951762</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="5"/>
-        <v>66.574839302112025</v>
+        <v>60.853432282003709</v>
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -893,31 +893,31 @@
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>99.068100358422939</v>
+        <v>89.847715736040598</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>87.813620071684582</v>
+        <v>75.465313028764797</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ref="F19:J19" si="6">F7*100</f>
-        <v>95.483870967741936</v>
+        <v>81.725888324873097</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="6"/>
-        <v>97.347670250896059</v>
+        <v>85.109983079526202</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="6"/>
-        <v>97.849462365591393</v>
+        <v>87.817258883248712</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="6"/>
-        <v>96.272401433691755</v>
+        <v>86.97123519458539</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="6"/>
-        <v>59.211469534050174</v>
+        <v>50.084602368866307</v>
       </c>
       <c r="K19" s="2"/>
     </row>

</xml_diff>

<commit_message>
latest confusion matrices and accuracies files
</commit_message>
<xml_diff>
--- a/figures/Table of Accuracies.xlsx
+++ b/figures/Table of Accuracies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabiki\Desktop\development\schmitz_r-lymphocyte_activation\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFD53AC-4341-4F6C-B365-8455A5264D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B3064B-9881-4E09-A6D6-F0B45E7A2582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60705" yWindow="9330" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="6660" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,18 +398,18 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1"/>
+    <col min="2" max="2" width="12.84375" customWidth="1"/>
+    <col min="3" max="3" width="41.3828125" customWidth="1"/>
+    <col min="4" max="4" width="10.53515625" bestFit="1"/>
+    <col min="10" max="10" width="11.69140625" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -476,7 +476,7 @@
         <v>0.63360881542699699</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -508,7 +508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -543,7 +543,7 @@
         <v>0.56029684601113094</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -575,7 +575,7 @@
         <v>0.34786641929499001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -607,7 +607,7 @@
         <v>0.60853432282003705</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -639,12 +639,12 @@
         <v>0.50084602368866304</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -679,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -719,7 +719,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -758,7 +758,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -801,7 +801,7 @@
         <v>56.029684601113097</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
updated confusion matrices and accuracies
</commit_message>
<xml_diff>
--- a/figures/Table of Accuracies.xlsx
+++ b/figures/Table of Accuracies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabiki\Desktop\development\schmitz_r-lymphocyte_activation\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B3064B-9881-4E09-A6D6-F0B45E7A2582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E0F638-218E-45E0-8186-D3D5149F1313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="6660" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,18 +398,18 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.84375" customWidth="1"/>
-    <col min="3" max="3" width="41.3828125" customWidth="1"/>
-    <col min="4" max="4" width="10.53515625" bestFit="1"/>
-    <col min="10" max="10" width="11.69140625" bestFit="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -476,7 +476,7 @@
         <v>0.63360881542699699</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -508,7 +508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -519,31 +519,31 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>0.90723562152133497</v>
+        <v>0.977621483375959</v>
       </c>
       <c r="E4">
-        <v>0.72634508348794002</v>
+        <v>0.85741687979539605</v>
       </c>
       <c r="F4">
-        <v>0.80612244897959096</v>
+        <v>0.906649616368286</v>
       </c>
       <c r="G4">
-        <v>0.82745825602968404</v>
+        <v>0.92838874680306904</v>
       </c>
       <c r="H4">
-        <v>0.86456400742115003</v>
+        <v>0.96419437340153402</v>
       </c>
       <c r="I4">
-        <v>0.86456400742115003</v>
+        <v>0.89897698209718602</v>
       </c>
       <c r="J4">
-        <v>0.50927643784786603</v>
+        <v>0.56329923273657201</v>
       </c>
       <c r="K4">
-        <v>0.56029684601113094</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.64002557544756999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -554,28 +554,28 @@
         <v>21</v>
       </c>
       <c r="D5">
-        <v>0.86085343228200295</v>
+        <v>0.90025575447570305</v>
       </c>
       <c r="E5">
-        <v>0.36549165120593602</v>
+        <v>0.50447570332480796</v>
       </c>
       <c r="F5">
-        <v>0.62523191094619601</v>
+        <v>0.74360613810741605</v>
       </c>
       <c r="G5">
-        <v>0.76066790352504599</v>
+        <v>0.81265984654731405</v>
       </c>
       <c r="H5">
-        <v>0.81632653061224403</v>
+        <v>0.83184143222506302</v>
       </c>
       <c r="I5">
-        <v>0.77272727272727204</v>
+        <v>0.83312020460358005</v>
       </c>
       <c r="J5">
-        <v>0.34786641929499001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.37020460358056201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -586,28 +586,28 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>0.92486085343228197</v>
+        <v>0.92199488491048598</v>
       </c>
       <c r="E6">
-        <v>0.67996289424860801</v>
+        <v>0.68734015345268495</v>
       </c>
       <c r="F6">
-        <v>0.84230055658627001</v>
+        <v>0.83759590792838801</v>
       </c>
       <c r="G6">
-        <v>0.87569573283859004</v>
+        <v>0.87851662404092001</v>
       </c>
       <c r="H6">
-        <v>0.90630797773654903</v>
+        <v>0.91432225063938599</v>
       </c>
       <c r="I6">
-        <v>0.90538033395176198</v>
+        <v>0.90345268542199397</v>
       </c>
       <c r="J6">
-        <v>0.60853432282003705</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.62020460358056195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -618,33 +618,33 @@
         <v>13</v>
       </c>
       <c r="D7">
-        <v>0.89847715736040601</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="E7">
-        <v>0.75465313028764802</v>
+        <v>0.873142857142857</v>
       </c>
       <c r="F7">
-        <v>0.81725888324873097</v>
+        <v>0.91314285714285703</v>
       </c>
       <c r="G7">
-        <v>0.85109983079526197</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="H7">
-        <v>0.87817258883248706</v>
+        <v>0.94628571428571395</v>
       </c>
       <c r="I7">
-        <v>0.86971235194585395</v>
+        <v>0.91542857142857104</v>
       </c>
       <c r="J7">
-        <v>0.50084602368866304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.54285714285714204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -679,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -719,7 +719,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -758,7 +758,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -770,38 +770,38 @@
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>90.723562152133496</v>
+        <v>97.762148337595903</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
-        <v>72.634508348794</v>
+        <v>85.741687979539606</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" ref="F16:K16" si="3">F4*100</f>
-        <v>80.612244897959101</v>
+        <v>90.664961636828593</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="3"/>
-        <v>82.745825602968409</v>
+        <v>92.838874680306901</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="3"/>
-        <v>86.456400742115008</v>
+        <v>96.419437340153408</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="3"/>
-        <v>86.456400742115008</v>
+        <v>89.897698209718598</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="3"/>
-        <v>50.927643784786603</v>
+        <v>56.329923273657201</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="3"/>
-        <v>56.029684601113097</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+        <v>64.002557544756996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -813,35 +813,35 @@
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>86.085343228200301</v>
+        <v>90.025575447570304</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>36.549165120593599</v>
+        <v>50.447570332480794</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" ref="F17:J17" si="4">F5*100</f>
-        <v>62.523191094619598</v>
+        <v>74.360613810741611</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="4"/>
-        <v>76.066790352504597</v>
+        <v>81.265984654731398</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="4"/>
-        <v>81.632653061224403</v>
+        <v>83.184143222506307</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="4"/>
-        <v>77.272727272727209</v>
+        <v>83.312020460357999</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="4"/>
-        <v>34.786641929498998</v>
+        <v>37.020460358056198</v>
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -853,35 +853,35 @@
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>92.486085343228197</v>
+        <v>92.199488491048598</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>67.996289424860805</v>
+        <v>68.734015345268489</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ref="F18:J18" si="5">F6*100</f>
-        <v>84.230055658626995</v>
+        <v>83.759590792838807</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="5"/>
-        <v>87.569573283859</v>
+        <v>87.851662404091996</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="5"/>
-        <v>90.630797773654905</v>
+        <v>91.432225063938603</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="5"/>
-        <v>90.5380333951762</v>
+        <v>90.345268542199392</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="5"/>
-        <v>60.853432282003709</v>
+        <v>62.020460358056198</v>
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -893,31 +893,31 @@
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>89.847715736040598</v>
+        <v>98.4</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>75.465313028764797</v>
+        <v>87.314285714285703</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ref="F19:J19" si="6">F7*100</f>
-        <v>81.725888324873097</v>
+        <v>91.314285714285703</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="6"/>
-        <v>85.109983079526202</v>
+        <v>94.399999999999991</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="6"/>
-        <v>87.817258883248712</v>
+        <v>94.628571428571391</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="6"/>
-        <v>86.97123519458539</v>
+        <v>91.542857142857102</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="6"/>
-        <v>50.084602368866307</v>
+        <v>54.285714285714207</v>
       </c>
       <c r="K19" s="2"/>
     </row>

</xml_diff>